<commit_message>
Update of the Statistical descriptions
</commit_message>
<xml_diff>
--- a/data/sample.xlsx
+++ b/data/sample.xlsx
@@ -1,34 +1,58 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Documents\X3\U.E_5_Traitement_de_données\Projet_DATA\projet-data\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B98410FF-73EF-425C-A5DE-F83C23915342}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+  <si>
+    <t>Vehicles_no</t>
+  </si>
+  <si>
+    <t>Iterations_no</t>
+  </si>
+  <si>
+    <t>Clients_no</t>
+  </si>
+  <si>
+    <t>Covered_dist</t>
+  </si>
+  <si>
+    <t>Convergence_Time</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -47,80 +71,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -408,893 +373,886 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" customWidth="1"/>
+    <col min="5" max="5" width="26.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Vehicles_no</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Iterations_no</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Clients_no</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Covered_dist</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>Convergence_Time</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
         <v>5</v>
       </c>
-      <c r="B2" t="n">
+      <c r="B2">
         <v>70</v>
       </c>
-      <c r="C2" t="n">
+      <c r="C2">
         <v>74</v>
       </c>
-      <c r="D2" t="n">
+      <c r="D2">
         <v>155</v>
       </c>
-      <c r="E2" t="n">
+      <c r="E2">
         <v>6.34</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="n">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
         <v>4</v>
       </c>
-      <c r="B3" t="n">
+      <c r="B3">
         <v>72</v>
       </c>
-      <c r="C3" t="n">
+      <c r="C3">
         <v>27</v>
       </c>
-      <c r="D3" t="n">
+      <c r="D3">
         <v>111</v>
       </c>
-      <c r="E3" t="n">
+      <c r="E3">
         <v>2.75</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="n">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>6</v>
       </c>
-      <c r="B4" t="n">
+      <c r="B4">
         <v>61</v>
       </c>
-      <c r="C4" t="n">
+      <c r="C4">
         <v>75</v>
       </c>
-      <c r="D4" t="n">
+      <c r="D4">
         <v>187</v>
       </c>
-      <c r="E4" t="n">
+      <c r="E4">
         <v>8.07</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="n">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
         <v>1</v>
       </c>
-      <c r="B5" t="n">
+      <c r="B5">
         <v>91</v>
       </c>
-      <c r="C5" t="n">
+      <c r="C5">
         <v>16</v>
       </c>
-      <c r="D5" t="n">
+      <c r="D5">
         <v>42</v>
       </c>
-      <c r="E5" t="n">
-        <v>1.16</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
+      <c r="E5">
+        <v>1.1599999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" t="n">
+      <c r="B6">
         <v>47</v>
       </c>
-      <c r="C6" t="n">
+      <c r="C6">
         <v>37</v>
       </c>
-      <c r="D6" t="n">
+      <c r="D6">
         <v>125</v>
       </c>
-      <c r="E6" t="n">
+      <c r="E6">
         <v>2.79</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="n">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
         <v>2</v>
       </c>
-      <c r="B7" t="n">
+      <c r="B7">
         <v>72</v>
       </c>
-      <c r="C7" t="n">
+      <c r="C7">
         <v>25</v>
       </c>
-      <c r="D7" t="n">
+      <c r="D7">
         <v>64</v>
       </c>
-      <c r="E7" t="n">
+      <c r="E7">
         <v>2.77</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="n">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
         <v>8</v>
       </c>
-      <c r="B8" t="n">
+      <c r="B8">
         <v>49</v>
       </c>
-      <c r="C8" t="n">
+      <c r="C8">
         <v>55</v>
       </c>
-      <c r="D8" t="n">
+      <c r="D8">
         <v>138</v>
       </c>
-      <c r="E8" t="n">
+      <c r="E8">
         <v>1</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" t="n">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
         <v>4</v>
       </c>
-      <c r="B9" t="n">
+      <c r="B9">
         <v>91</v>
       </c>
-      <c r="C9" t="n">
+      <c r="C9">
         <v>25</v>
       </c>
-      <c r="D9" t="n">
+      <c r="D9">
         <v>87</v>
       </c>
-      <c r="E9" t="n">
+      <c r="E9">
         <v>2.08</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" t="n">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
         <v>3</v>
       </c>
-      <c r="B10" t="n">
+      <c r="B10">
         <v>49</v>
       </c>
-      <c r="C10" t="n">
+      <c r="C10">
         <v>25</v>
       </c>
-      <c r="D10" t="n">
+      <c r="D10">
         <v>78</v>
       </c>
-      <c r="E10" t="n">
+      <c r="E10">
         <v>2.62</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" t="n">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
         <v>4</v>
       </c>
-      <c r="B11" t="n">
+      <c r="B11">
         <v>70</v>
       </c>
-      <c r="C11" t="n">
+      <c r="C11">
         <v>48</v>
       </c>
-      <c r="D11" t="n">
+      <c r="D11">
         <v>126</v>
       </c>
-      <c r="E11" t="n">
+      <c r="E11">
         <v>0.97</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" t="n">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
         <v>1</v>
       </c>
-      <c r="B12" t="n">
+      <c r="B12">
         <v>74</v>
       </c>
-      <c r="C12" t="n">
+      <c r="C12">
         <v>4</v>
       </c>
-      <c r="D12" t="n">
+      <c r="D12">
         <v>14</v>
       </c>
-      <c r="E12" t="n">
+      <c r="E12">
         <v>0.52</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" t="n">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
         <v>9</v>
       </c>
-      <c r="B13" t="n">
+      <c r="B13">
         <v>49</v>
       </c>
-      <c r="C13" t="n">
+      <c r="C13">
         <v>109</v>
       </c>
-      <c r="D13" t="n">
+      <c r="D13">
         <v>321</v>
       </c>
-      <c r="E13" t="n">
+      <c r="E13">
         <v>2.78</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" t="n">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
         <v>3</v>
       </c>
-      <c r="B14" t="n">
+      <c r="B14">
         <v>78</v>
       </c>
-      <c r="C14" t="n">
+      <c r="C14">
         <v>10</v>
       </c>
-      <c r="D14" t="n">
+      <c r="D14">
         <v>43</v>
       </c>
-      <c r="E14" t="n">
+      <c r="E14">
         <v>1.19</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" t="n">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
         <v>10</v>
       </c>
-      <c r="B15" t="n">
+      <c r="B15">
         <v>57</v>
       </c>
-      <c r="C15" t="n">
+      <c r="C15">
         <v>66</v>
       </c>
-      <c r="D15" t="n">
+      <c r="D15">
         <v>288</v>
       </c>
-      <c r="E15" t="n">
+      <c r="E15">
         <v>7.69</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" t="n">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
         <v>1</v>
       </c>
-      <c r="B16" t="n">
+      <c r="B16">
         <v>75</v>
       </c>
-      <c r="C16" t="n">
+      <c r="C16">
         <v>3</v>
       </c>
-      <c r="D16" t="n">
+      <c r="D16">
         <v>16</v>
       </c>
-      <c r="E16" t="n">
-        <v>0.14</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="n">
+      <c r="E16">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17">
         <v>1</v>
       </c>
-      <c r="B17" t="n">
+      <c r="B17">
         <v>64</v>
       </c>
-      <c r="C17" t="n">
+      <c r="C17">
         <v>8</v>
       </c>
-      <c r="D17" t="n">
+      <c r="D17">
         <v>23</v>
       </c>
-      <c r="E17" t="n">
+      <c r="E17">
         <v>0.27</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" t="n">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18">
         <v>2</v>
       </c>
-      <c r="B18" t="n">
+      <c r="B18">
         <v>79</v>
       </c>
-      <c r="C18" t="n">
+      <c r="C18">
         <v>19</v>
       </c>
-      <c r="D18" t="n">
+      <c r="D18">
         <v>45</v>
       </c>
-      <c r="E18" t="n">
-        <v>0.55</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="n">
+      <c r="E18">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19">
         <v>3</v>
       </c>
-      <c r="B19" t="n">
+      <c r="B19">
         <v>73</v>
       </c>
-      <c r="C19" t="n">
+      <c r="C19">
         <v>11</v>
       </c>
-      <c r="D19" t="n">
+      <c r="D19">
         <v>60</v>
       </c>
-      <c r="E19" t="n">
+      <c r="E19">
         <v>1.04</v>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" t="n">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20">
         <v>10</v>
       </c>
-      <c r="B20" t="n">
+      <c r="B20">
         <v>42</v>
       </c>
-      <c r="C20" t="n">
+      <c r="C20">
         <v>112</v>
       </c>
-      <c r="D20" t="n">
+      <c r="D20">
         <v>290</v>
       </c>
-      <c r="E20" t="n">
+      <c r="E20">
         <v>6.71</v>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" t="n">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21">
         <v>9</v>
       </c>
-      <c r="B21" t="n">
+      <c r="B21">
         <v>94</v>
       </c>
-      <c r="C21" t="n">
+      <c r="C21">
         <v>97</v>
       </c>
-      <c r="D21" t="n">
+      <c r="D21">
         <v>223</v>
       </c>
-      <c r="E21" t="n">
+      <c r="E21">
         <v>15.23</v>
       </c>
     </row>
-    <row r="22">
-      <c r="A22" t="n">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22">
         <v>6</v>
       </c>
-      <c r="B22" t="n">
+      <c r="B22">
         <v>35</v>
       </c>
-      <c r="C22" t="n">
+      <c r="C22">
         <v>74</v>
       </c>
-      <c r="D22" t="n">
+      <c r="D22">
         <v>240</v>
       </c>
-      <c r="E22" t="n">
+      <c r="E22">
         <v>1.04</v>
       </c>
     </row>
-    <row r="23">
-      <c r="A23" t="n">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23">
         <v>7</v>
       </c>
-      <c r="B23" t="n">
+      <c r="B23">
         <v>66</v>
       </c>
-      <c r="C23" t="n">
+      <c r="C23">
         <v>25</v>
       </c>
-      <c r="D23" t="n">
+      <c r="D23">
         <v>164</v>
       </c>
-      <c r="E23" t="n">
+      <c r="E23">
         <v>4.32</v>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" t="n">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24">
         <v>6</v>
       </c>
-      <c r="B24" t="n">
+      <c r="B24">
         <v>43</v>
       </c>
-      <c r="C24" t="n">
+      <c r="C24">
         <v>31</v>
       </c>
-      <c r="D24" t="n">
+      <c r="D24">
         <v>120</v>
       </c>
-      <c r="E24" t="n">
+      <c r="E24">
         <v>3.48</v>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" t="n">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25">
         <v>4</v>
       </c>
-      <c r="B25" t="n">
+      <c r="B25">
         <v>93</v>
       </c>
-      <c r="C25" t="n">
+      <c r="C25">
         <v>56</v>
       </c>
-      <c r="D25" t="n">
+      <c r="D25">
         <v>137</v>
       </c>
-      <c r="E25" t="n">
+      <c r="E25">
         <v>7.27</v>
       </c>
     </row>
-    <row r="26">
-      <c r="A26" t="n">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26">
         <v>4</v>
       </c>
-      <c r="B26" t="n">
+      <c r="B26">
         <v>68</v>
       </c>
-      <c r="C26" t="n">
+      <c r="C26">
         <v>56</v>
       </c>
-      <c r="D26" t="n">
+      <c r="D26">
         <v>144</v>
       </c>
-      <c r="E26" t="n">
-        <v>4.85</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="n">
+      <c r="E26">
+        <v>4.8499999999999996</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27">
         <v>10</v>
       </c>
-      <c r="B27" t="n">
+      <c r="B27">
         <v>37</v>
       </c>
-      <c r="C27" t="n">
+      <c r="C27">
         <v>114</v>
       </c>
-      <c r="D27" t="n">
+      <c r="D27">
         <v>442</v>
       </c>
-      <c r="E27" t="n">
+      <c r="E27">
         <v>1.58</v>
       </c>
     </row>
-    <row r="28">
-      <c r="A28" t="n">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28">
         <v>6</v>
       </c>
-      <c r="B28" t="n">
+      <c r="B28">
         <v>35</v>
       </c>
-      <c r="C28" t="n">
+      <c r="C28">
         <v>77</v>
       </c>
-      <c r="D28" t="n">
+      <c r="D28">
         <v>227</v>
       </c>
-      <c r="E28" t="n">
+      <c r="E28">
         <v>3.21</v>
       </c>
     </row>
-    <row r="29">
-      <c r="A29" t="n">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29">
         <v>10</v>
       </c>
-      <c r="B29" t="n">
+      <c r="B29">
         <v>61</v>
       </c>
-      <c r="C29" t="n">
+      <c r="C29">
         <v>30</v>
       </c>
-      <c r="D29" t="n">
+      <c r="D29">
         <v>129</v>
       </c>
-      <c r="E29" t="n">
-        <v>2.28</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="n">
+      <c r="E29">
+        <v>2.2799999999999998</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30">
         <v>9</v>
       </c>
-      <c r="B30" t="n">
+      <c r="B30">
         <v>78</v>
       </c>
-      <c r="C30" t="n">
+      <c r="C30">
         <v>133</v>
       </c>
-      <c r="D30" t="n">
+      <c r="D30">
         <v>381</v>
       </c>
-      <c r="E30" t="n">
+      <c r="E30">
         <v>3.12</v>
       </c>
     </row>
-    <row r="31">
-      <c r="A31" t="n">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31">
         <v>10</v>
       </c>
-      <c r="B31" t="n">
+      <c r="B31">
         <v>86</v>
       </c>
-      <c r="C31" t="n">
+      <c r="C31">
         <v>128</v>
       </c>
-      <c r="D31" t="n">
+      <c r="D31">
         <v>332</v>
       </c>
-      <c r="E31" t="n">
+      <c r="E31">
         <v>6.6</v>
       </c>
     </row>
-    <row r="32">
-      <c r="A32" t="n">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32">
         <v>1</v>
       </c>
-      <c r="B32" t="n">
+      <c r="B32">
         <v>67</v>
       </c>
-      <c r="C32" t="n">
+      <c r="C32">
         <v>17</v>
       </c>
-      <c r="D32" t="n">
+      <c r="D32">
         <v>54</v>
       </c>
-      <c r="E32" t="n">
+      <c r="E32">
         <v>0.52</v>
       </c>
     </row>
-    <row r="33">
-      <c r="A33" t="n">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33">
         <v>2</v>
       </c>
-      <c r="B33" t="n">
+      <c r="B33">
         <v>48</v>
       </c>
-      <c r="C33" t="n">
+      <c r="C33">
         <v>23</v>
       </c>
-      <c r="D33" t="n">
+      <c r="D33">
         <v>84</v>
       </c>
-      <c r="E33" t="n">
+      <c r="E33">
         <v>0.67</v>
       </c>
     </row>
-    <row r="34">
-      <c r="A34" t="n">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34">
         <v>7</v>
       </c>
-      <c r="B34" t="n">
+      <c r="B34">
         <v>86</v>
       </c>
-      <c r="C34" t="n">
+      <c r="C34">
         <v>29</v>
       </c>
-      <c r="D34" t="n">
+      <c r="D34">
         <v>158</v>
       </c>
-      <c r="E34" t="n">
+      <c r="E34">
         <v>1.86</v>
       </c>
     </row>
-    <row r="35">
-      <c r="A35" t="n">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35">
         <v>8</v>
       </c>
-      <c r="B35" t="n">
+      <c r="B35">
         <v>98</v>
       </c>
-      <c r="C35" t="n">
+      <c r="C35">
         <v>70</v>
       </c>
-      <c r="D35" t="n">
+      <c r="D35">
         <v>277</v>
       </c>
-      <c r="E35" t="n">
+      <c r="E35">
         <v>9.77</v>
       </c>
     </row>
-    <row r="36">
-      <c r="A36" t="n">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36">
         <v>9</v>
       </c>
-      <c r="B36" t="n">
+      <c r="B36">
         <v>89</v>
       </c>
-      <c r="C36" t="n">
+      <c r="C36">
         <v>66</v>
       </c>
-      <c r="D36" t="n">
+      <c r="D36">
         <v>274</v>
       </c>
-      <c r="E36" t="n">
+      <c r="E36">
         <v>7.02</v>
       </c>
     </row>
-    <row r="37">
-      <c r="A37" t="n">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37">
         <v>7</v>
       </c>
-      <c r="B37" t="n">
+      <c r="B37">
         <v>62</v>
       </c>
-      <c r="C37" t="n">
+      <c r="C37">
         <v>68</v>
       </c>
-      <c r="D37" t="n">
+      <c r="D37">
         <v>144</v>
       </c>
-      <c r="E37" t="n">
+      <c r="E37">
         <v>1.47</v>
       </c>
     </row>
-    <row r="38">
-      <c r="A38" t="n">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38">
         <v>8</v>
       </c>
-      <c r="B38" t="n">
+      <c r="B38">
         <v>65</v>
       </c>
-      <c r="C38" t="n">
+      <c r="C38">
         <v>107</v>
       </c>
-      <c r="D38" t="n">
+      <c r="D38">
         <v>240</v>
       </c>
-      <c r="E38" t="n">
+      <c r="E38">
         <v>14.19</v>
       </c>
     </row>
-    <row r="39">
-      <c r="A39" t="n">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39">
         <v>6</v>
       </c>
-      <c r="B39" t="n">
+      <c r="B39">
         <v>61</v>
       </c>
-      <c r="C39" t="n">
+      <c r="C39">
         <v>52</v>
       </c>
-      <c r="D39" t="n">
+      <c r="D39">
         <v>156</v>
       </c>
-      <c r="E39" t="n">
+      <c r="E39">
         <v>3.11</v>
       </c>
     </row>
-    <row r="40">
-      <c r="A40" t="n">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40">
         <v>9</v>
       </c>
-      <c r="B40" t="n">
+      <c r="B40">
         <v>87</v>
       </c>
-      <c r="C40" t="n">
+      <c r="C40">
         <v>99</v>
       </c>
-      <c r="D40" t="n">
+      <c r="D40">
         <v>289</v>
       </c>
-      <c r="E40" t="n">
+      <c r="E40">
         <v>3.86</v>
       </c>
     </row>
-    <row r="41">
-      <c r="A41" t="n">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41">
         <v>7</v>
       </c>
-      <c r="B41" t="n">
+      <c r="B41">
         <v>30</v>
       </c>
-      <c r="C41" t="n">
+      <c r="C41">
         <v>39</v>
       </c>
-      <c r="D41" t="n">
+      <c r="D41">
         <v>204</v>
       </c>
-      <c r="E41" t="n">
-        <v>1.16</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="n">
+      <c r="E41">
+        <v>1.1599999999999999</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42">
         <v>9</v>
       </c>
-      <c r="B42" t="n">
+      <c r="B42">
         <v>47</v>
       </c>
-      <c r="C42" t="n">
+      <c r="C42">
         <v>37</v>
       </c>
-      <c r="D42" t="n">
+      <c r="D42">
         <v>195</v>
       </c>
-      <c r="E42" t="n">
+      <c r="E42">
         <v>1.82</v>
       </c>
     </row>
-    <row r="43">
-      <c r="A43" t="n">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43">
         <v>2</v>
       </c>
-      <c r="B43" t="n">
+      <c r="B43">
         <v>82</v>
       </c>
-      <c r="C43" t="n">
+      <c r="C43">
         <v>19</v>
       </c>
-      <c r="D43" t="n">
+      <c r="D43">
         <v>49</v>
       </c>
-      <c r="E43" t="n">
+      <c r="E43">
         <v>1.78</v>
       </c>
     </row>
-    <row r="44">
-      <c r="A44" t="n">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44">
         <v>8</v>
       </c>
-      <c r="B44" t="n">
+      <c r="B44">
         <v>41</v>
       </c>
-      <c r="C44" t="n">
+      <c r="C44">
         <v>48</v>
       </c>
-      <c r="D44" t="n">
+      <c r="D44">
         <v>135</v>
       </c>
-      <c r="E44" t="n">
+      <c r="E44">
         <v>1.49</v>
       </c>
     </row>
-    <row r="45">
-      <c r="A45" t="n">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45">
         <v>4</v>
       </c>
-      <c r="B45" t="n">
+      <c r="B45">
         <v>31</v>
       </c>
-      <c r="C45" t="n">
+      <c r="C45">
         <v>44</v>
       </c>
-      <c r="D45" t="n">
+      <c r="D45">
         <v>111</v>
       </c>
-      <c r="E45" t="n">
+      <c r="E45">
         <v>0.61</v>
       </c>
     </row>
-    <row r="46">
-      <c r="A46" t="n">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46">
         <v>4</v>
       </c>
-      <c r="B46" t="n">
+      <c r="B46">
         <v>97</v>
       </c>
-      <c r="C46" t="n">
+      <c r="C46">
         <v>30</v>
       </c>
-      <c r="D46" t="n">
+      <c r="D46">
         <v>123</v>
       </c>
-      <c r="E46" t="n">
+      <c r="E46">
         <v>3.65</v>
       </c>
     </row>
-    <row r="47">
-      <c r="A47" t="n">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47">
         <v>2</v>
       </c>
-      <c r="B47" t="n">
+      <c r="B47">
         <v>82</v>
       </c>
-      <c r="C47" t="n">
+      <c r="C47">
         <v>25</v>
       </c>
-      <c r="D47" t="n">
+      <c r="D47">
         <v>60</v>
       </c>
-      <c r="E47" t="n">
+      <c r="E47">
         <v>1.42</v>
       </c>
     </row>
-    <row r="48">
-      <c r="A48" t="n">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48">
         <v>1</v>
       </c>
-      <c r="B48" t="n">
+      <c r="B48">
         <v>57</v>
       </c>
-      <c r="C48" t="n">
+      <c r="C48">
         <v>9</v>
       </c>
-      <c r="D48" t="n">
+      <c r="D48">
         <v>26</v>
       </c>
-      <c r="E48" t="n">
+      <c r="E48">
         <v>0.27</v>
       </c>
     </row>
-    <row r="49">
-      <c r="A49" t="n">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49">
         <v>10</v>
       </c>
-      <c r="B49" t="n">
+      <c r="B49">
         <v>95</v>
       </c>
-      <c r="C49" t="n">
+      <c r="C49">
         <v>140</v>
       </c>
-      <c r="D49" t="n">
+      <c r="D49">
         <v>421</v>
       </c>
-      <c r="E49" t="n">
+      <c r="E49">
         <v>21.51</v>
       </c>
     </row>
-    <row r="50">
-      <c r="A50" t="n">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50">
         <v>3</v>
       </c>
-      <c r="B50" t="n">
+      <c r="B50">
         <v>63</v>
       </c>
-      <c r="C50" t="n">
+      <c r="C50">
         <v>33</v>
       </c>
-      <c r="D50" t="n">
+      <c r="D50">
         <v>101</v>
       </c>
-      <c r="E50" t="n">
+      <c r="E50">
         <v>0.95</v>
       </c>
     </row>
-    <row r="51">
-      <c r="A51" t="n">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51">
         <v>2</v>
       </c>
-      <c r="B51" t="n">
+      <c r="B51">
         <v>45</v>
       </c>
-      <c r="C51" t="n">
+      <c r="C51">
         <v>22</v>
       </c>
-      <c r="D51" t="n">
+      <c r="D51">
         <v>64</v>
       </c>
-      <c r="E51" t="n">
+      <c r="E51">
         <v>1.21</v>
       </c>
     </row>

</xml_diff>